<commit_message>
WID - Sanity checks
Mostly checking which distributions have all the 130 quantiles queried in Stata
</commit_message>
<xml_diff>
--- a/PabloArriagada/poverty_inequality_dataexplorer/WID/Percentile names.xlsx
+++ b/PabloArriagada/poverty_inequality_dataexplorer/WID/Percentile names.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\Google Drive\OWID\notebooks\poverty_inequality_dataexplorer\WID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\Google Drive OWID\notebooks\PabloArriagada\poverty_inequality_dataexplorer\WID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58357560-7AFB-4B3D-9FA0-C4B95F17079E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3391B0F4-6E43-483D-8A12-86416DC8F7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{850EDBB3-6C12-4D21-9CAD-062574D9D5A7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="258">
   <si>
     <t>p0</t>
   </si>
@@ -800,13 +800,22 @@
   </si>
   <si>
     <t>p99.999p100</t>
+  </si>
+  <si>
+    <t>p99p100</t>
+  </si>
+  <si>
+    <t>p99.9p100</t>
+  </si>
+  <si>
+    <t>p99.99p100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -816,6 +825,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -841,8 +857,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1157,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A94EBB-AF1D-4315-97E1-31F35AB56513}">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C127"/>
+      <selection activeCell="C1" sqref="C1:C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +1970,7 @@
         <v>66</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C127" si="1">A66&amp;B66</f>
+        <f t="shared" ref="C66:C130" si="1">A66&amp;B66</f>
         <v>p65p66</v>
       </c>
     </row>
@@ -2354,337 +2371,373 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B100" t="s">
-        <v>101</v>
-      </c>
-      <c r="C100" t="str">
-        <f t="shared" si="1"/>
-        <v>p99p99.1</v>
+      <c r="B100" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C100" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>p99p100</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
         <v>101</v>
       </c>
-      <c r="B101" t="s">
-        <v>102</v>
-      </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>p99.1p99.2</v>
+        <v>p99p99.1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>102</v>
       </c>
-      <c r="B102" t="s">
-        <v>103</v>
-      </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v>p99.2p99.3</v>
+        <v>p99.1p99.2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
         <v>103</v>
       </c>
-      <c r="B103" t="s">
-        <v>104</v>
-      </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v>p99.3p99.4</v>
+        <v>p99.2p99.3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
         <v>104</v>
       </c>
-      <c r="B104" t="s">
-        <v>105</v>
-      </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v>p99.4p99.5</v>
+        <v>p99.3p99.4</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
         <v>105</v>
       </c>
-      <c r="B105" t="s">
-        <v>106</v>
-      </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v>p99.5p99.6</v>
+        <v>p99.4p99.5</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" t="s">
-        <v>107</v>
-      </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v>p99.6p99.7</v>
+        <v>p99.5p99.6</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" t="s">
-        <v>108</v>
-      </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>p99.7p99.8</v>
+        <v>p99.6p99.7</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
         <v>108</v>
       </c>
-      <c r="B108" t="s">
-        <v>109</v>
-      </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v>p99.8p99.9</v>
+        <v>p99.7p99.8</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
         <v>109</v>
       </c>
-      <c r="B109" t="s">
-        <v>110</v>
-      </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v>p99.9p99.91</v>
+        <v>p99.8p99.9</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>110</v>
-      </c>
-      <c r="B110" t="s">
-        <v>111</v>
-      </c>
-      <c r="C110" t="str">
-        <f t="shared" si="1"/>
-        <v>p99.91p99.92</v>
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C110" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>p99.9p100</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>p99.92p99.93</v>
+        <v>p99.9p99.91</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>p99.93p99.94</v>
+        <v>p99.91p99.92</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
-        <v>p99.94p99.95</v>
+        <v>p99.92p99.93</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v>p99.95p99.96</v>
+        <v>p99.93p99.94</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v>p99.96p99.97</v>
+        <v>p99.94p99.95</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v>p99.97p99.98</v>
+        <v>p99.95p99.96</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v>p99.98p99.99</v>
+        <v>p99.96p99.97</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
-        <v>p99.99p99.991</v>
+        <v>p99.97p99.98</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>p99.991p99.992</v>
+        <v>p99.98p99.99</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>120</v>
-      </c>
-      <c r="B120" t="s">
-        <v>121</v>
-      </c>
-      <c r="C120" t="str">
-        <f t="shared" si="1"/>
-        <v>p99.992p99.993</v>
+      <c r="A120" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C120" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>p99.99p100</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
-        <v>p99.993p99.994</v>
+        <v>p99.99p99.991</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
-        <v>p99.994p99.995</v>
+        <v>p99.991p99.992</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
-        <v>p99.995p99.996</v>
+        <v>p99.992p99.993</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
-        <v>p99.996p99.997</v>
+        <v>p99.993p99.994</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
-        <v>p99.997p99.998</v>
+        <v>p99.994p99.995</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
-        <v>p99.998p99.999</v>
+        <v>p99.995p99.996</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>124</v>
+      </c>
+      <c r="B127" t="s">
+        <v>125</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>p99.996p99.997</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>125</v>
+      </c>
+      <c r="B128" t="s">
+        <v>126</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>p99.997p99.998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>126</v>
+      </c>
+      <c r="B129" t="s">
         <v>127</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>p99.998p99.999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C127" t="str">
+      <c r="C130" s="1" t="str">
         <f t="shared" si="1"/>
         <v>p99.999p100</v>
       </c>
@@ -2692,20 +2745,21 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A27042-264C-4807-90F3-6ED32E8E1F89}">
-  <dimension ref="A1:DW1"/>
+  <dimension ref="A1:DZ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="DD1" workbookViewId="0">
+      <selection sqref="A1:DZ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:127" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:130" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -3003,88 +3057,97 @@
       <c r="CU1" t="s">
         <v>226</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CV1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="CW1" t="s">
         <v>227</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>228</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>229</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>230</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>231</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>232</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>233</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>234</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>235</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="DG1" t="s">
         <v>236</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DH1" t="s">
         <v>237</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DI1" t="s">
         <v>238</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DJ1" t="s">
         <v>239</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DK1" t="s">
         <v>240</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DL1" t="s">
         <v>241</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DM1" t="s">
         <v>242</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DN1" t="s">
         <v>243</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DO1" t="s">
         <v>244</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DP1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="DQ1" t="s">
         <v>245</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DR1" t="s">
         <v>246</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DS1" t="s">
         <v>247</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DT1" t="s">
         <v>248</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DU1" t="s">
         <v>249</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DV1" t="s">
         <v>250</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DW1" t="s">
         <v>251</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DX1" t="s">
         <v>252</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DY1" t="s">
         <v>253</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DZ1" s="1" t="s">
         <v>254</v>
       </c>
     </row>

</xml_diff>